<commit_message>
Se agrega contenido para manejo de datos creando utilidad data driven
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Documents\Selenium2Unidad\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0B5668-7307-432B-88AD-094A920F7462}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCB8AB9-2F99-449A-AFCC-E35A370959EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{B5BB45CF-8E8F-4FBA-9BB1-E75EE45CC37F}"/>
   </bookViews>
@@ -127,13 +127,13 @@
     <t>CP001_Error_creacion_Cta_problema_tecnico</t>
   </si>
   <si>
-    <t>41177071-0</t>
-  </si>
-  <si>
     <t>correovalido@algo.com</t>
   </si>
   <si>
     <t>Tenemos un problema técnico</t>
+  </si>
+  <si>
+    <t>23635557-8</t>
   </si>
 </sst>
 </file>
@@ -571,112 +571,138 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D279F09-04AD-4C55-85EB-77C419C0646F}">
-  <dimension ref="B2:P17"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+    <row r="2" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D2" s="3">
+        <v>87645876</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="3">
-        <v>87645876</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -685,11 +711,13 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>29</v>
@@ -697,22 +725,38 @@
       <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>29</v>
@@ -732,26 +776,20 @@
       <c r="H6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>29</v>
@@ -765,42 +803,30 @@
       <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -809,11 +835,13 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>29</v>
@@ -821,22 +849,38 @@
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>29</v>
@@ -856,26 +900,20 @@
       <c r="H10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>29</v>
@@ -889,42 +927,30 @@
       <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -933,11 +959,13 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>29</v>
@@ -945,10 +973,18 @@
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -956,11 +992,13 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>29</v>
@@ -974,42 +1012,30 @@
       <c r="F14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1018,11 +1044,13 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>29</v>
@@ -1030,69 +1058,43 @@
       <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P17" s="1" t="s">
+      <c r="E16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{E553729B-389D-4972-BBE7-F20E4D1A244C}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E553729B-389D-4972-BBE7-F20E4D1A244C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Se actualiza el proyecto con el contenido de properties manager
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Data.xlsx
+++ b/src/test/resources/data/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Documents\Selenium2Unidad\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCB8AB9-2F99-449A-AFCC-E35A370959EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600BAB0B-55A6-48A0-B303-A089F6618C69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="3" xr2:uid="{B5BB45CF-8E8F-4FBA-9BB1-E75EE45CC37F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="33">
   <si>
     <t>CasosDePrueba</t>
   </si>
@@ -130,10 +130,7 @@
     <t>correovalido@algo.com</t>
   </si>
   <si>
-    <t>Tenemos un problema técnico</t>
-  </si>
-  <si>
-    <t>23635557-8</t>
+    <t>El Rut ingresado no es válido</t>
   </si>
 </sst>
 </file>
@@ -574,7 +571,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,8 +634,8 @@
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>33</v>
+      <c r="B2" s="3">
+        <v>123122222</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>31</v>

</xml_diff>